<commit_message>
grafica con paralelismo cuerpos+coordenadas
</commit_message>
<xml_diff>
--- a/graficas Secuencial vs OpenMP (4 y 8 hilos)/IC OpenMP.xlsx
+++ b/graficas Secuencial vs OpenMP (4 y 8 hilos)/IC OpenMP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t>Secuencial</t>
   </si>
@@ -26,13 +26,19 @@
   <si>
     <t>8 hilos</t>
   </si>
+  <si>
+    <t>8 hilos(cuerpos+coordenadas)</t>
+  </si>
+  <si>
+    <t>8 hilos (cuerpos+coordenadas)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -66,7 +72,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,7 +116,23 @@
                   <a:schemeClr val="bg1"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>20 cuerpos</a:t>
+              <a:t>5 cuerpos (comparativa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> con </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>paralelismo de cuerpos y cálculo de X e Y)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -119,8 +141,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.41468599983272131"/>
-          <c:y val="1.8408229299861599E-2"/>
+          <c:x val="0.1818671252310996"/>
+          <c:y val="2.6048716785604997E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -140,7 +162,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$K$1</c:f>
+              <c:f>Hoja1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -152,60 +174,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$13:$A$19</c:f>
+              <c:f>Hoja1!$A$12:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2097152</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8388608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$K$13:$K$19</c:f>
+              <c:f>Hoja1!$E$12:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.5629999999999999</c:v>
+                  <c:v>0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1190000000000002</c:v>
+                  <c:v>0.379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2069999999999999</c:v>
+                  <c:v>0.76500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.377000000000001</c:v>
+                  <c:v>1.5609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.856999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>49.686</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>99.281999999999996</c:v>
+                  <c:v>3.0950000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -216,7 +226,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$L$1</c:f>
+              <c:f>Hoja1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -228,60 +238,48 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$13:$A$19</c:f>
+              <c:f>Hoja1!$A$12:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2097152</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8388608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$L$13:$L$19</c:f>
+              <c:f>Hoja1!$F$12:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.67200000000000004</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.298</c:v>
+                  <c:v>0.219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6320000000000001</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1929999999999996</c:v>
+                  <c:v>0.85899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.217000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.594000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42.878</c:v>
+                  <c:v>1.6659999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,7 +290,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$M$1</c:f>
+              <c:f>Hoja1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -304,60 +302,112 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$13:$A$19</c:f>
+              <c:f>Hoja1!$A$12:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2097152</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8388608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$M$13:$M$19</c:f>
+              <c:f>Hoja1!$G$12:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.59699999999999998</c:v>
+                  <c:v>7.8E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2350000000000001</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4129999999999998</c:v>
+                  <c:v>0.35099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.72</c:v>
+                  <c:v>0.68799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.4860000000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.068999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38.779000000000003</c:v>
+                  <c:v>1.355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 hilos (cuerpos+coordenadas)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$12:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$H$12:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.21199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3980000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,11 +422,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="57478528"/>
-        <c:axId val="57877248"/>
+        <c:axId val="158360320"/>
+        <c:axId val="158362240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57478528"/>
+        <c:axId val="158360320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +491,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57877248"/>
+        <c:crossAx val="158362240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -449,7 +499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57877248"/>
+        <c:axId val="158362240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +555,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -523,7 +573,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57478528"/>
+        <c:crossAx val="158360320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -581,14 +631,31 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88867865268614976"/>
-          <c:y val="0.4549085036885393"/>
-          <c:w val="0.10589643913000381"/>
-          <c:h val="0.17511126779713224"/>
+          <c:x val="0.74494431459538646"/>
+          <c:y val="0.37595721188188069"/>
+          <c:w val="0.25505568540461343"/>
+          <c:h val="0.23348169039617633"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -625,15 +692,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>330572</xdr:colOff>
+      <xdr:colOff>357786</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
+      <xdr:rowOff>53628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>408214</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>100854</xdr:rowOff>
+      <xdr:rowOff>87246</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -942,15 +1009,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -970,43 +1037,49 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
       <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
-        <v>0</v>
-      </c>
       <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" t="s">
-        <v>0</v>
-      </c>
       <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
         <v>1</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>64</v>
       </c>
@@ -1028,9 +1101,7 @@
       <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2">
         <v>0</v>
       </c>
@@ -1050,22 +1121,28 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
         <v>1E-3</v>
       </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
       <c r="Q2" s="2">
         <v>0</v>
       </c>
       <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>128</v>
       </c>
@@ -1087,9 +1164,7 @@
       <c r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2">
         <v>0</v>
       </c>
@@ -1109,22 +1184,28 @@
         <v>0</v>
       </c>
       <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
         <v>2E-3</v>
       </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
       <c r="Q3" s="2">
         <v>0</v>
       </c>
       <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>256</v>
       </c>
@@ -1146,9 +1227,7 @@
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2">
         <v>0</v>
       </c>
@@ -1168,22 +1247,28 @@
         <v>0</v>
       </c>
       <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
       <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="S4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1512</v>
       </c>
@@ -1205,9 +1290,7 @@
       <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2">
         <v>0</v>
       </c>
@@ -1224,25 +1307,31 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
       <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1024</v>
       </c>
@@ -1264,44 +1353,48 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
       <c r="J6" s="2">
         <v>0</v>
       </c>
       <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
       <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <v>2E-3</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>6.2E-2</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6" s="2">
+        <v>1.054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2048</v>
       </c>
@@ -1323,44 +1416,48 @@
       <c r="G7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
         <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J7" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K7" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L7" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>0.126</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U7" s="2">
+        <v>2.1190000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4096</v>
       </c>
@@ -1382,44 +1479,48 @@
       <c r="G8" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>6.3E-2</v>
-      </c>
-      <c r="L8" s="2">
-        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M8" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="N8" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O8" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>0.23400000000000001</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>0.111</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>9.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8" s="2">
+        <v>4.3789999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8192</v>
       </c>
@@ -1441,44 +1542,48 @@
       <c r="G9" s="2">
         <v>0.02</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>0.20300000000000001</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>0.105</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>7.8E-2</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>0.48</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>0.23400000000000001</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9" s="2">
+        <v>8.6449999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16384</v>
       </c>
@@ -1500,44 +1605,48 @@
       <c r="G10" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
         <v>0.10299999999999999</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4.7E-2</v>
       </c>
       <c r="J10" s="2">
         <v>4.7E-2</v>
       </c>
       <c r="K10" s="2">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L10" s="2">
         <v>0.187</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>7.8E-2</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>0.375</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>0.20300000000000001</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>0.95799999999999996</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>0.47599999999999998</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>0.35899999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10" s="2">
+        <v>17.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32768</v>
       </c>
@@ -1559,44 +1668,48 @@
       <c r="G11" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
         <v>0.188</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>7.8E-2</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>0.39100000000000001</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>0.17199999999999999</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>0.157</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>0.78600000000000003</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>0.41</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>0.29699999999999999</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>1.9419999999999999</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>0.94699999999999995</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>0.76600000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11" s="2">
+        <v>34.527999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>65536</v>
       </c>
@@ -1619,43 +1732,49 @@
         <v>7.8E-2</v>
       </c>
       <c r="H12" s="2">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I12" s="2">
         <v>0.39</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>0.187</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>0.17199999999999999</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>0.78100000000000003</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>0.32800000000000001</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>0.28100000000000003</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>1.55</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>0.754</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>0.56599999999999995</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="R12" s="2">
         <v>3.8420000000000001</v>
       </c>
-      <c r="R12" s="2">
+      <c r="S12" s="2">
         <v>1.7949999999999999</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>1.4530000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12" s="2">
+        <v>69.998000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>131072</v>
       </c>
@@ -1678,43 +1797,49 @@
         <v>0.156</v>
       </c>
       <c r="H13" s="2">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="I13" s="2">
         <v>0.77300000000000002</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>0.36</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>0.34100000000000003</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>1.5629999999999999</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>0.67200000000000004</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>0.59699999999999998</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>3.1179999999999999</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>1.5129999999999999</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>1.206</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>7.7359999999999998</v>
       </c>
-      <c r="R13" s="2">
+      <c r="S13" s="2">
         <v>3.6030000000000002</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>2.9359999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="2">
+        <v>137.86000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>262144</v>
       </c>
@@ -1737,43 +1862,49 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="H14" s="2">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="I14" s="2">
         <v>1.5469999999999999</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>0.71799999999999997</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>0.68700000000000006</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>3.1190000000000002</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>1.298</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>1.2350000000000001</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>6.2130000000000001</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>3.0089999999999999</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>2.3639999999999999</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>15.398</v>
       </c>
-      <c r="R14" s="2">
+      <c r="S14" s="2">
         <v>7.7069999999999999</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>6.077</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" s="2">
+        <v>282.339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>524288</v>
       </c>
@@ -1796,43 +1927,49 @@
         <v>0.68799999999999994</v>
       </c>
       <c r="H15" s="2">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="I15" s="2">
         <v>3.1230000000000002</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>1.4219999999999999</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>1.391</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>6.2069999999999999</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>2.6320000000000001</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>2.4129999999999998</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>12.391</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>6.3419999999999996</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>4.657</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>30.718</v>
       </c>
-      <c r="R15" s="2">
+      <c r="S15" s="2">
         <v>14.975</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <v>12.064</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="2">
+        <v>545.00699999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1048576</v>
       </c>
@@ -1855,43 +1992,46 @@
         <v>1.355</v>
       </c>
       <c r="H16" s="2">
+        <v>2.3980000000000001</v>
+      </c>
+      <c r="I16" s="2">
         <v>6.202</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>2.8119999999999998</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>2.7829999999999999</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>12.377000000000001</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>5.1929999999999996</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>4.72</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>24.756</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <v>11.881</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>9.1259999999999994</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>61.889000000000003</v>
       </c>
-      <c r="R16" s="2">
+      <c r="S16" s="2">
         <v>30.364000000000001</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <v>23.535</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2097152</v>
       </c>
@@ -1913,44 +2053,45 @@
       <c r="G17" s="2">
         <v>2.5230000000000001</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
         <v>12.423999999999999</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>5.6829999999999998</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>5.4379999999999997</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>24.856999999999999</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>10.217000000000001</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>9.4860000000000007</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <v>49.332000000000001</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2">
         <v>23.27</v>
       </c>
-      <c r="P17" s="2">
+      <c r="Q17" s="2">
         <v>18.18</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="R17" s="2">
         <v>126.96899999999999</v>
       </c>
-      <c r="R17" s="2">
+      <c r="S17" s="2">
         <v>61.459000000000003</v>
       </c>
-      <c r="S17" s="2">
+      <c r="T17" s="2">
         <v>46.387999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4194304</v>
       </c>
@@ -1972,44 +2113,45 @@
       <c r="G18" s="2">
         <v>5.4880000000000004</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2">
         <v>24.855</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>11.968999999999999</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>11.045</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>49.686</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>20.594000000000001</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>19.068999999999999</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <v>98.668000000000006</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <v>48.537999999999997</v>
       </c>
-      <c r="P18" s="2">
+      <c r="Q18" s="2">
         <v>35.573999999999998</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="R18" s="2">
         <v>246.71700000000001</v>
       </c>
-      <c r="R18" s="2">
+      <c r="S18" s="2">
         <v>125.598</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <v>95.084999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8388608</v>
       </c>
@@ -2031,41 +2173,50 @@
       <c r="G19" s="2">
         <v>11.256</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
         <v>49.741</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>23.838999999999999</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>22.32</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>99.281999999999996</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M19" s="2">
         <v>42.878</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <v>38.779000000000003</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>197.09700000000001</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <v>101.60899999999999</v>
       </c>
-      <c r="P19" s="2">
+      <c r="Q19" s="2">
         <v>76.628</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="R19" s="2">
         <v>555.09400000000005</v>
       </c>
-      <c r="R19" s="2">
+      <c r="S19" s="2">
         <v>253.54900000000001</v>
       </c>
-      <c r="S19" s="2">
+      <c r="T19" s="2">
         <v>186.72800000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H21" s="2">
+        <v>107.711</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>